<commit_message>
created new log structure and updated filepath to return appropriate log info
</commit_message>
<xml_diff>
--- a/btsAccountsTest10.xlsx
+++ b/btsAccountsTest10.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Production" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Production" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>7-8</t>
   </si>
@@ -92,9 +96,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,11 +106,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,19 +146,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -164,10 +167,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -323,7 +326,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -332,13 +335,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -348,7 +351,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -357,7 +360,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -366,7 +369,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -376,12 +379,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -412,7 +415,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -431,7 +434,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -443,212 +446,215 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col width="9.10" min="1" max="1"/>
-    <col width="9.10" min="2" max="2"/>
-    <col width="9.10" min="3" max="3"/>
-    <col width="9.10" min="4" max="4"/>
-    <col width="9.10" min="5" max="5"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:5" r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:5" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="C2">
-        <v>20</v>
-      </c>
-      <c t="s" r="D2">
-        <v>12</v>
-      </c>
-      <c t="s" r="E2">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:5" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:5">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="C3">
-        <v>20</v>
-      </c>
-      <c t="s" r="D3">
-        <v>12</v>
-      </c>
-      <c t="s" r="E3">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:5" r="4">
-      <c t="n" r="A4">
+    <row r="4" spans="1:5">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="C4">
-        <v>20</v>
-      </c>
-      <c t="s" r="D4">
-        <v>12</v>
-      </c>
-      <c t="s" r="E4">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row spans="1:5" r="5">
-      <c t="n" r="A5">
+    <row r="5" spans="1:5">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="C5">
-        <v>20</v>
-      </c>
-      <c t="s" r="D5">
-        <v>12</v>
-      </c>
-      <c t="s" r="E5">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:5" r="6">
-      <c t="n" r="A6">
+    <row r="6" spans="1:5">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="C6">
-        <v>20</v>
-      </c>
-      <c t="s" r="D6">
-        <v>12</v>
-      </c>
-      <c t="s" r="E6">
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row spans="1:5" r="7">
-      <c t="n" r="A7">
+    <row r="7" spans="1:5">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="C7">
-        <v>20</v>
-      </c>
-      <c t="s" r="D7">
-        <v>12</v>
-      </c>
-      <c t="s" r="E7">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:5" r="8">
-      <c t="n" r="A8">
+    <row r="8" spans="1:5">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="C8">
-        <v>20</v>
-      </c>
-      <c t="s" r="D8">
-        <v>12</v>
-      </c>
-      <c t="s" r="E8">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row spans="1:5" r="9">
-      <c t="n" r="A9">
+    <row r="9" spans="1:5">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="C9">
-        <v>20</v>
-      </c>
-      <c t="s" r="D9">
-        <v>12</v>
-      </c>
-      <c t="s" r="E9">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:5" r="10">
-      <c t="n" r="A10">
+    <row r="10" spans="1:5">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C10">
-        <v>20</v>
-      </c>
-      <c t="s" r="D10">
-        <v>12</v>
-      </c>
-      <c t="s" r="E10">
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:5" r="11">
-      <c t="n" r="A11">
+    <row r="11" spans="1:5">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C11">
-        <v>20</v>
-      </c>
-      <c t="s" r="D11">
-        <v>12</v>
-      </c>
-      <c t="s" r="E11">
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
player selection now happens in units of 20, to be more fault tolerant. It also only updates those players that haven't already been updated today
</commit_message>
<xml_diff>
--- a/btsAccountsTest10.xlsx
+++ b/btsAccountsTest10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24220" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>7-8</t>
   </si>
@@ -91,13 +91,19 @@
   </si>
   <si>
     <t>williams.daft.741@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>VM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +118,37 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -121,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -144,17 +181,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E11"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -459,10 +528,12 @@
     <col min="2" max="2" width="41.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="4" customWidth="1"/>
+    <col min="7" max="7" width="68.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -475,11 +546,17 @@
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -492,11 +569,17 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -509,11 +592,17 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -526,11 +615,17 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -543,11 +638,17 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>4</v>
       </c>
@@ -560,11 +661,17 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -577,11 +684,17 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
@@ -594,11 +707,17 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -611,11 +730,17 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
@@ -628,11 +753,17 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
@@ -645,12 +776,19 @@
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>